<commit_message>
Selenium project with POM and TestNG and Maven and Datadriven - 2nd Commit
</commit_message>
<xml_diff>
--- a/src/main/java/com/pom/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/pom/qa/testdata/FreeCrmTestData.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MuraliJavaProjects\PomTestNGMaven\src\main\java\com\pom\qa\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{028FAECF-57E9-43A0-A14D-8A0EBB5E4F73}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{999268C6-5135-4EEA-85DC-0277B9BBFEA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="4896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>firstname</t>
   </si>
@@ -38,9 +34,6 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Pom</t>
   </si>
   <si>
@@ -48,6 +41,15 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Testing2</t>
+  </si>
+  <si>
+    <t>Testing3</t>
+  </si>
+  <si>
+    <t>Testing4</t>
   </si>
 </sst>
 </file>
@@ -383,7 +385,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -398,26 +400,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>